<commit_message>
Revise the Activity1 excel file
</commit_message>
<xml_diff>
--- a/Activity1/Activity1.xlsx
+++ b/Activity1/Activity1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbroman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbroman/Docs/Talks/RRworkshop/Activity1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,8 +106,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,7 +132,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -139,6 +141,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -147,6 +150,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,34 +426,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="1">
-        <v>42648</v>
-      </c>
-      <c r="C1" s="1">
-        <v>42655</v>
-      </c>
-      <c r="D1" s="1">
-        <v>42662</v>
-      </c>
-      <c r="E1" s="1">
-        <v>42648</v>
-      </c>
-      <c r="F1" s="1">
-        <v>42655</v>
-      </c>
-      <c r="G1" s="1">
-        <v>42662</v>
-      </c>
-    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
@@ -464,107 +448,147 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>146.6</v>
-      </c>
-      <c r="C4">
-        <v>138.6</v>
-      </c>
-      <c r="D4">
-        <v>155.6</v>
-      </c>
-      <c r="E4">
-        <v>166</v>
-      </c>
-      <c r="F4">
-        <v>179.3</v>
-      </c>
-      <c r="G4">
-        <v>186.9</v>
+      <c r="B4" s="1">
+        <v>42648</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42655</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42662</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42648</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42655</v>
+      </c>
+      <c r="G4" s="1">
+        <v>42662</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>146.6</v>
+      </c>
+      <c r="C5">
+        <v>138.6</v>
+      </c>
+      <c r="D5">
+        <v>155.6</v>
+      </c>
+      <c r="E5">
+        <v>166</v>
+      </c>
+      <c r="F5">
+        <v>179.3</v>
+      </c>
+      <c r="G5">
+        <v>186.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>245.7</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>240</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>243.1</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>177.8</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>171.6</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>188.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>42648</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42655</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42662</v>
+      </c>
+      <c r="E10" s="1">
+        <v>42648</v>
+      </c>
+      <c r="F10" s="1">
+        <v>42655</v>
+      </c>
+      <c r="G10" s="1">
+        <v>42662</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>333.6</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>353.6</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>408.8</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <v>450.6</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>474.4</v>
       </c>
-      <c r="G9">
+      <c r="G11">
         <v>423.8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>514.4</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>610.6</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>597.9</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>412.1</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <v>447.4</v>
       </c>
-      <c r="G10">
+      <c r="G12">
         <v>446.5</v>
       </c>
     </row>

</xml_diff>